<commit_message>
Total number of domain's count
Total number of domain's count
</commit_message>
<xml_diff>
--- a/analysis/queryResults/Number_of_Configurations_per_Domain_results_02022018_afterRemoving_NULL_ERR.xlsx
+++ b/analysis/queryResults/Number_of_Configurations_per_Domain_results_02022018_afterRemoving_NULL_ERR.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malik\Documents\GitHub\AnalyzeServerConfigurationBehaviour\analysis\queryResults\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malik\Google Drive\analysis\queryResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Number_of_Configurations_per_Do" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -613,7 +613,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -702,7 +701,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -891,8 +889,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-157105008"/>
-        <c:axId val="-157113168"/>
+        <c:axId val="397271840"/>
+        <c:axId val="397261504"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -1080,7 +1078,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-157105008"/>
+        <c:axId val="397271840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1122,7 +1120,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-157113168"/>
+        <c:crossAx val="397261504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1130,7 +1128,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-157113168"/>
+        <c:axId val="397261504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1181,7 +1179,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-157105008"/>
+        <c:crossAx val="397271840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2071,16 +2069,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B67"/>
+  <dimension ref="A1:B68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D3" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B51"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" customWidth="1"/>
+    <col min="1" max="1" width="33.42578125" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -2619,6 +2617,12 @@
         <v>1</v>
       </c>
     </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B68">
+        <f>SUM(B2:B67)</f>
+        <v>58327</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>